<commit_message>
Chinh dua giao dien, gop file excel
</commit_message>
<xml_diff>
--- a/dat/2008-09-07.xlsx
+++ b/dat/2008-09-07.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="IT_B" sheetId="1" r:id="rId1"/>
@@ -758,7 +758,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -793,7 +793,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1002,9 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -1908,6 +1909,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1996,9 +1998,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>

</xml_diff>